<commit_message>
Nome das colunas atualizados
</commit_message>
<xml_diff>
--- a/coca.xlsx
+++ b/coca.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RF\Downloads\P2_Ciencia_dos_dados\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Downloads\Insper\2 Semestre\Ciencia_dos_Dados\P2_Ciencia_dos_dados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7FD4E0F-517D-4874-B893-5F9CB1C8FA6B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8D34592-EBF0-4197-A107-AF2ABAD01ECC}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2304" yWindow="2304" windowWidth="13824" windowHeight="7152" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Treinamento" sheetId="2" r:id="rId1"/>
@@ -3195,9 +3195,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3208,7 +3206,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>2</v>
@@ -9971,9 +9969,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -9984,7 +9980,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>2</v>

</xml_diff>

<commit_message>
coluna simulação no excel
</commit_message>
<xml_diff>
--- a/coca.xlsx
+++ b/coca.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Downloads\Insper\2 Semestre\Ciencia_dos_Dados\P2_Ciencia_dos_dados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8D34592-EBF0-4197-A107-AF2ABAD01ECC}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27EDB780-B5C2-40F6-BDE4-CB6D8D9A39AF}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1004" uniqueCount="898">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1005" uniqueCount="899">
   <si>
     <t>Treinamento</t>
   </si>
@@ -2887,12 +2887,15 @@
   <si>
     <t>hoje eu só quero água e coca-cola .. 👎</t>
   </si>
+  <si>
+    <t>Simulação</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2923,6 +2926,14 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="major"/>
     </font>
   </fonts>
   <fills count="2">
@@ -2960,7 +2971,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -2976,6 +2987,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -9967,26 +9981,32 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B1000"/>
+  <dimension ref="A1:C1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="154" customWidth="1"/>
     <col min="2" max="2" width="18.5" customWidth="1"/>
-    <col min="3" max="26" width="7.59765625" customWidth="1"/>
+    <col min="3" max="3" width="12.3984375" customWidth="1"/>
+    <col min="4" max="26" width="7.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C1" s="7" t="s">
+        <v>898</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
@@ -9994,7 +10014,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
@@ -10002,7 +10022,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>7</v>
       </c>
@@ -10010,7 +10030,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>9</v>
       </c>
@@ -10018,7 +10038,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>11</v>
       </c>
@@ -10026,7 +10046,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>13</v>
       </c>
@@ -10034,7 +10054,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>16</v>
       </c>
@@ -10042,7 +10062,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>18</v>
       </c>
@@ -10050,7 +10070,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>21</v>
       </c>
@@ -10058,7 +10078,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>24</v>
       </c>
@@ -10066,7 +10086,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>27</v>
       </c>
@@ -10074,7 +10094,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>28</v>
       </c>
@@ -10082,7 +10102,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>29</v>
       </c>
@@ -10090,7 +10110,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>32</v>
       </c>
@@ -10098,7 +10118,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>35</v>
       </c>
@@ -14235,6 +14255,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>